<commit_message>
Afegida funció formula_text() amb millores
</commit_message>
<xml_diff>
--- a/data/conductor_test.xlsx
+++ b/data/conductor_test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
@@ -11,8 +11,70 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>Sepal.Length</t>
+  </si>
+  <si>
+    <t>camp</t>
+  </si>
+  <si>
+    <t>Petal.Length</t>
+  </si>
+  <si>
+    <t>Petal.Width</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Sepal.Width</t>
+  </si>
+  <si>
+    <t>etiqueta</t>
+  </si>
+  <si>
+    <t>formula</t>
+  </si>
+  <si>
+    <t>Lengh Sepal</t>
+  </si>
+  <si>
+    <t>Widht of Sepal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lengh of petal </t>
+  </si>
+  <si>
+    <t>Widht of Petal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Species varies </t>
+  </si>
+  <si>
+    <t>recode</t>
+  </si>
+  <si>
+    <t>rank</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>Catalonia</t>
+  </si>
+  <si>
+    <t>regiligio</t>
+  </si>
+  <si>
+    <t>fsffadf</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -46,8 +108,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -60,7 +125,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Oficina">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -98,7 +163,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Oficina">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -168,7 +233,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Oficina">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -342,12 +407,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="5" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>

</xml_diff>